<commit_message>
chore: apply line ending fixes to documentation files
Automated Formatting:
- Fixed line endings in markdown documentation
- Normalized end-of-file formatting
- Applied to configuration and backup files

Files affected (documentation only):
- *.md files - line ending normalization
- *.backup files - formatting consistency
- *.sh scripts - line ending fixes
- *.xlsx test outputs - binary updates
- *.pdf test fixtures - binary updates

No functional changes to source code.

Impact:
- ✅ Consistent line endings across documentation
- ✅ Improved cross-platform compatibility
- ✅ Clean pre-commit hook compliance for docs
</commit_message>
<xml_diff>
--- a/tests/outputs/test_daily_details_thick_borders.xlsx
+++ b/tests/outputs/test_daily_details_thick_borders.xlsx
@@ -33,7 +33,6 @@
       <color rgb="00000000"/>
     </font>
     <font>
-      <b val="1"/>
       <sz val="11"/>
     </font>
   </fonts>
@@ -211,10 +210,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
@@ -740,7 +743,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45871</v>
+        <v>45931</v>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
@@ -804,7 +807,7 @@
       </c>
       <c r="V2" s="3" t="inlineStr">
         <is>
-          <t>2025-08-02|CX1|Driver 1|BW1</t>
+          <t>2025-10-01|CX1|Driver 1|BW1</t>
         </is>
       </c>
       <c r="W2" s="3" t="inlineStr"/>
@@ -812,7 +815,7 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="n">
-        <v>45871</v>
+        <v>45931</v>
       </c>
       <c r="B3" s="6" t="inlineStr">
         <is>
@@ -876,7 +879,7 @@
       </c>
       <c r="V3" s="6" t="inlineStr">
         <is>
-          <t>2025-08-02|CX2|Driver 2|BW2</t>
+          <t>2025-10-01|CX2|Driver 2|BW2</t>
         </is>
       </c>
       <c r="W3" s="6" t="inlineStr"/>
@@ -884,7 +887,7 @@
     </row>
     <row r="4">
       <c r="A4" s="5" t="n">
-        <v>45871</v>
+        <v>45931</v>
       </c>
       <c r="B4" s="6" t="inlineStr">
         <is>
@@ -948,7 +951,7 @@
       </c>
       <c r="V4" s="6" t="inlineStr">
         <is>
-          <t>2025-08-02|CX3|Driver 3|BW3</t>
+          <t>2025-10-01|CX3|Driver 3|BW3</t>
         </is>
       </c>
       <c r="W4" s="6" t="inlineStr"/>
@@ -956,7 +959,7 @@
     </row>
     <row r="5">
       <c r="A5" s="5" t="n">
-        <v>45871</v>
+        <v>45931</v>
       </c>
       <c r="B5" s="6" t="inlineStr">
         <is>
@@ -1020,7 +1023,7 @@
       </c>
       <c r="V5" s="6" t="inlineStr">
         <is>
-          <t>2025-08-02|CX4|Driver 4|BW4</t>
+          <t>2025-10-01|CX4|Driver 4|BW4</t>
         </is>
       </c>
       <c r="W5" s="6" t="inlineStr"/>
@@ -1028,7 +1031,7 @@
     </row>
     <row r="6">
       <c r="A6" s="8" t="n">
-        <v>45871</v>
+        <v>45931</v>
       </c>
       <c r="B6" s="9" t="inlineStr">
         <is>
@@ -1092,7 +1095,7 @@
       </c>
       <c r="V6" s="9" t="inlineStr">
         <is>
-          <t>2025-08-02|CX5|Driver 5|BW5</t>
+          <t>2025-10-01|CX5|Driver 5|BW5</t>
         </is>
       </c>
       <c r="W6" s="9" t="inlineStr"/>
@@ -1100,7 +1103,7 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45872</v>
+        <v>45932</v>
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
@@ -1165,7 +1168,7 @@
       </c>
       <c r="W7" s="3" t="inlineStr">
         <is>
-          <t>2025-08-03|CX10|Driver 10|BW10</t>
+          <t>2025-10-02|CX10|Driver 10|BW10</t>
         </is>
       </c>
       <c r="X7" s="4" t="inlineStr"/>
@@ -1173,7 +1176,7 @@
     </row>
     <row r="8">
       <c r="A8" s="5" t="n">
-        <v>45872</v>
+        <v>45932</v>
       </c>
       <c r="B8" s="6" t="inlineStr">
         <is>
@@ -1238,7 +1241,7 @@
       </c>
       <c r="W8" s="6" t="inlineStr">
         <is>
-          <t>2025-08-03|CX11|Driver 11|BW11</t>
+          <t>2025-10-02|CX11|Driver 11|BW11</t>
         </is>
       </c>
       <c r="X8" s="7" t="inlineStr"/>
@@ -1246,7 +1249,7 @@
     </row>
     <row r="9">
       <c r="A9" s="8" t="n">
-        <v>45872</v>
+        <v>45932</v>
       </c>
       <c r="B9" s="9" t="inlineStr">
         <is>
@@ -1311,7 +1314,7 @@
       </c>
       <c r="W9" s="9" t="inlineStr">
         <is>
-          <t>2025-08-03|CX12|Driver 12|BW12</t>
+          <t>2025-10-02|CX12|Driver 12|BW12</t>
         </is>
       </c>
       <c r="X9" s="10" t="inlineStr"/>
@@ -1319,7 +1322,7 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>45873</v>
+        <v>45933</v>
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
@@ -1384,7 +1387,7 @@
       </c>
       <c r="W10" s="3" t="inlineStr">
         <is>
-          <t>2025-08-04|CX20|Driver 20|BW20</t>
+          <t>2025-10-03|CX20|Driver 20|BW20</t>
         </is>
       </c>
       <c r="X10" s="4" t="inlineStr"/>
@@ -1392,7 +1395,7 @@
     </row>
     <row r="11">
       <c r="A11" s="5" t="n">
-        <v>45873</v>
+        <v>45933</v>
       </c>
       <c r="B11" s="6" t="inlineStr">
         <is>
@@ -1457,7 +1460,7 @@
       </c>
       <c r="W11" s="6" t="inlineStr">
         <is>
-          <t>2025-08-04|CX21|Driver 21|BW21</t>
+          <t>2025-10-03|CX21|Driver 21|BW21</t>
         </is>
       </c>
       <c r="X11" s="7" t="inlineStr"/>
@@ -1465,7 +1468,7 @@
     </row>
     <row r="12">
       <c r="A12" s="5" t="n">
-        <v>45873</v>
+        <v>45933</v>
       </c>
       <c r="B12" s="6" t="inlineStr">
         <is>
@@ -1530,7 +1533,7 @@
       </c>
       <c r="W12" s="6" t="inlineStr">
         <is>
-          <t>2025-08-04|CX22|Driver 22|BW22</t>
+          <t>2025-10-03|CX22|Driver 22|BW22</t>
         </is>
       </c>
       <c r="X12" s="7" t="inlineStr"/>
@@ -1538,7 +1541,7 @@
     </row>
     <row r="13">
       <c r="A13" s="8" t="n">
-        <v>45873</v>
+        <v>45933</v>
       </c>
       <c r="B13" s="9" t="inlineStr">
         <is>
@@ -1603,7 +1606,7 @@
       </c>
       <c r="W13" s="9" t="inlineStr">
         <is>
-          <t>2025-08-04|CX23|Driver 23|BW23</t>
+          <t>2025-10-03|CX23|Driver 23|BW23</t>
         </is>
       </c>
       <c r="X13" s="10" t="inlineStr"/>

</xml_diff>